<commit_message>
Updated metrics for Iteration 5
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
+++ b/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
@@ -15,6 +15,9 @@
     <sheet name="Schedule Metrics Tracking" sheetId="12" r:id="rId1"/>
     <sheet name="Guidelines for Schedule Metrics" sheetId="11" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -915,37 +918,37 @@
                   <c:v>41946</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41960</c:v>
+                  <c:v>41988</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41974</c:v>
+                  <c:v>42002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41988</c:v>
+                  <c:v>42016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42002</c:v>
+                  <c:v>42030</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42016</c:v>
+                  <c:v>42044</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42030</c:v>
+                  <c:v>42058</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42044</c:v>
+                  <c:v>42072</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42058</c:v>
+                  <c:v>42086</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42072</c:v>
+                  <c:v>42100</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42086</c:v>
+                  <c:v>42114</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42100</c:v>
+                  <c:v>42128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1172,11 +1175,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="349256960"/>
-        <c:axId val="349257504"/>
+        <c:axId val="-813914064"/>
+        <c:axId val="-813899920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="349256960"/>
+        <c:axId val="-813914064"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1219,7 +1222,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349257504"/>
+        <c:crossAx val="-813899920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1227,7 +1230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349257504"/>
+        <c:axId val="-813899920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -1279,7 +1282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349256960"/>
+        <c:crossAx val="-813914064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -1483,37 +1486,37 @@
                   <c:v>41946</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41960</c:v>
+                  <c:v>41988</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41974</c:v>
+                  <c:v>42002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41988</c:v>
+                  <c:v>42016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42002</c:v>
+                  <c:v>42030</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42016</c:v>
+                  <c:v>42044</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42030</c:v>
+                  <c:v>42058</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42044</c:v>
+                  <c:v>42072</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42058</c:v>
+                  <c:v>42086</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42072</c:v>
+                  <c:v>42100</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42086</c:v>
+                  <c:v>42114</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42100</c:v>
+                  <c:v>42128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1629,7 +1632,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -1740,11 +1743,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="349261856"/>
-        <c:axId val="123162336"/>
+        <c:axId val="-820918912"/>
+        <c:axId val="-820905856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="349261856"/>
+        <c:axId val="-820918912"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1787,7 +1790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="123162336"/>
+        <c:crossAx val="-820905856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1795,7 +1798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123162336"/>
+        <c:axId val="-820905856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -1847,7 +1850,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349261856"/>
+        <c:crossAx val="-820918912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -3039,6 +3042,19 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Schedule Metrics"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3357,8 +3373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,7 +3479,7 @@
         <v>41918</v>
       </c>
       <c r="H5" s="12">
-        <f t="shared" ref="H5:H7" si="1">G5+13</f>
+        <f t="shared" ref="H5:H6" si="1">G5+13</f>
         <v>41931</v>
       </c>
       <c r="I5" s="10">
@@ -3558,26 +3574,30 @@
         <v>21</v>
       </c>
       <c r="C8" s="12">
-        <f t="shared" si="2"/>
-        <v>41960</v>
+        <v>41988</v>
       </c>
       <c r="D8" s="12">
         <f t="shared" si="0"/>
-        <v>41973</v>
+        <v>42001</v>
       </c>
       <c r="E8" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
         <v>14</v>
       </c>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="G8" s="12">
+        <v>41988</v>
+      </c>
+      <c r="H8" s="12">
+        <f>G8+13+1</f>
+        <v>42002</v>
+      </c>
       <c r="I8" s="10">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J8" s="11">
         <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="K8" s="10"/>
     </row>
@@ -3587,11 +3607,11 @@
       </c>
       <c r="C9" s="12">
         <f t="shared" si="2"/>
-        <v>41974</v>
+        <v>42002</v>
       </c>
       <c r="D9" s="12">
         <f t="shared" si="0"/>
-        <v>41987</v>
+        <v>42015</v>
       </c>
       <c r="E9" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3615,11 +3635,11 @@
       </c>
       <c r="C10" s="12">
         <f t="shared" si="2"/>
-        <v>41988</v>
+        <v>42016</v>
       </c>
       <c r="D10" s="12">
         <f t="shared" si="0"/>
-        <v>42001</v>
+        <v>42029</v>
       </c>
       <c r="E10" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3643,11 +3663,11 @@
       </c>
       <c r="C11" s="12">
         <f t="shared" si="2"/>
-        <v>42002</v>
+        <v>42030</v>
       </c>
       <c r="D11" s="12">
         <f t="shared" si="0"/>
-        <v>42015</v>
+        <v>42043</v>
       </c>
       <c r="E11" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3671,11 +3691,11 @@
       </c>
       <c r="C12" s="12">
         <f t="shared" si="2"/>
-        <v>42016</v>
+        <v>42044</v>
       </c>
       <c r="D12" s="12">
         <f t="shared" si="0"/>
-        <v>42029</v>
+        <v>42057</v>
       </c>
       <c r="E12" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3699,11 +3719,11 @@
       </c>
       <c r="C13" s="12">
         <f t="shared" si="2"/>
-        <v>42030</v>
+        <v>42058</v>
       </c>
       <c r="D13" s="12">
         <f t="shared" si="0"/>
-        <v>42043</v>
+        <v>42071</v>
       </c>
       <c r="E13" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3727,11 +3747,11 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" si="2"/>
-        <v>42044</v>
+        <v>42072</v>
       </c>
       <c r="D14" s="12">
         <f t="shared" si="0"/>
-        <v>42057</v>
+        <v>42085</v>
       </c>
       <c r="E14" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3755,11 +3775,11 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" si="2"/>
-        <v>42058</v>
+        <v>42086</v>
       </c>
       <c r="D15" s="12">
         <f t="shared" si="0"/>
-        <v>42071</v>
+        <v>42099</v>
       </c>
       <c r="E15" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3785,11 +3805,11 @@
       </c>
       <c r="C16" s="12">
         <f t="shared" si="2"/>
-        <v>42072</v>
+        <v>42100</v>
       </c>
       <c r="D16" s="12">
         <f t="shared" si="0"/>
-        <v>42085</v>
+        <v>42113</v>
       </c>
       <c r="E16" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3813,11 +3833,11 @@
       </c>
       <c r="C17" s="12">
         <f t="shared" si="2"/>
-        <v>42086</v>
+        <v>42114</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" si="0"/>
-        <v>42099</v>
+        <v>42127</v>
       </c>
       <c r="E17" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
@@ -3843,11 +3863,11 @@
       </c>
       <c r="C18" s="12">
         <f t="shared" si="2"/>
-        <v>42100</v>
+        <v>42128</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" si="0"/>
-        <v>42113</v>
+        <v>42141</v>
       </c>
       <c r="E18" s="10">
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>

</xml_diff>

<commit_message>
Updated iteration 6 metrics
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
+++ b/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Action</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>Schedule Metrics Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delayed slightly due to debugging phase, team was unfamiliar with charts. Date/time issue. Date showed NaN. </t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -380,7 +386,43 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1175,11 +1217,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-813914064"/>
-        <c:axId val="-813899920"/>
+        <c:axId val="-1664024672"/>
+        <c:axId val="-1380287328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-813914064"/>
+        <c:axId val="-1664024672"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1222,7 +1264,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-813899920"/>
+        <c:crossAx val="-1380287328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1230,7 +1272,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-813899920"/>
+        <c:axId val="-1380287328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -1282,7 +1324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-813914064"/>
+        <c:crossAx val="-1664024672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -1635,7 +1677,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -1743,11 +1785,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-820918912"/>
-        <c:axId val="-820905856"/>
+        <c:axId val="-1380287872"/>
+        <c:axId val="-1380290592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-820918912"/>
+        <c:axId val="-1380287872"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1790,7 +1832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-820905856"/>
+        <c:crossAx val="-1380290592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1798,7 +1840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-820905856"/>
+        <c:axId val="-1380290592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -1850,7 +1892,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-820918912"/>
+        <c:crossAx val="-1380287872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -1932,6 +1974,355 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG" sz="3600">
+                <a:latin typeface="Bebas Neue" panose="020B0606020202050201" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Schedule Metrics</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Schedule Metrics Tracking'!$J$4:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0769230769230769</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1380286240"/>
+        <c:axId val="-1380282976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1380286240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1380282976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1380282976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1380286240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
   <a:schemeClr val="dk1"/>
@@ -1965,6 +2356,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -2971,6 +3402,508 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3041,6 +3974,100 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>84753</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>149370</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>21648</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>86592</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18876818" y="4572001"/>
+          <a:ext cx="16774824" cy="4723532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:alpha val="8000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:alpha val="13000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3058,27 +4085,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:K18" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="B3:K18"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="Iteration" dataDxfId="9"/>
-    <tableColumn id="2" name="Planned Start Date" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:L18" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="B3:L18"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Iteration" dataDxfId="10"/>
+    <tableColumn id="2" name="Planned Start Date" dataDxfId="9">
       <calculatedColumnFormula>D3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Planned End Date" dataDxfId="7">
+    <tableColumn id="3" name="Planned End Date" dataDxfId="8">
       <calculatedColumnFormula>C4+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Duration (Days)" dataDxfId="6">
+    <tableColumn id="6" name="Duration (Days)" dataDxfId="7">
       <calculatedColumnFormula>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Milestone included" dataDxfId="5"/>
-    <tableColumn id="5" name="Actual Start Date" dataDxfId="4"/>
-    <tableColumn id="7" name="Actual End Date" dataDxfId="3"/>
-    <tableColumn id="8" name="Actual Duration (Days)" dataDxfId="2"/>
-    <tableColumn id="10" name="Schedule Metrics Score" dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="4" name="Milestone included" dataDxfId="6"/>
+    <tableColumn id="5" name="Actual Start Date" dataDxfId="5"/>
+    <tableColumn id="7" name="Actual End Date" dataDxfId="4"/>
+    <tableColumn id="8" name="Actual Duration (Days)" dataDxfId="3"/>
+    <tableColumn id="10" name="Schedule Metrics Score" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Action" dataDxfId="0"/>
+    <tableColumn id="9" name="Action" dataDxfId="1"/>
+    <tableColumn id="11" name="Remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3371,10 +4399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L18" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,10 +4417,11 @@
     <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="103.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3423,8 +4452,11 @@
       <c r="K3" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="L3" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
@@ -3456,8 +4488,9 @@
       <c r="K4" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
@@ -3492,8 +4525,9 @@
       <c r="K5" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
@@ -3530,8 +4564,9 @@
       <c r="K6" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
@@ -3568,8 +4603,9 @@
       <c r="K7" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>21</v>
       </c>
@@ -3599,9 +4635,14 @@
         <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
         <v>0.93333333333333335</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
@@ -3618,18 +4659,27 @@
         <v>14</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="G9" s="12">
+        <f t="shared" ref="G9" si="4">H8+1</f>
+        <v>42003</v>
+      </c>
+      <c r="H9" s="12">
+        <f t="shared" ref="H9" si="5">G9+13</f>
+        <v>42016</v>
+      </c>
       <c r="I9" s="10">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J9" s="11">
         <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
-      </c>
-      <c r="K9" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
@@ -3651,13 +4701,11 @@
       <c r="I10" s="10">
         <v>1</v>
       </c>
-      <c r="J10" s="11">
-        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
-      </c>
+      <c r="J10" s="11"/>
       <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
@@ -3679,13 +4727,11 @@
       <c r="I11" s="10">
         <v>1</v>
       </c>
-      <c r="J11" s="11">
-        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
-      </c>
+      <c r="J11" s="11"/>
       <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>25</v>
       </c>
@@ -3701,19 +4747,19 @@
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
         <v>14</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10">
         <v>1</v>
       </c>
-      <c r="J12" s="11">
-        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
-      </c>
+      <c r="J12" s="11"/>
       <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>26</v>
       </c>
@@ -3735,13 +4781,11 @@
       <c r="I13" s="10">
         <v>1</v>
       </c>
-      <c r="J13" s="11">
-        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
-      </c>
+      <c r="J13" s="11"/>
       <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
         <v>27</v>
       </c>
@@ -3763,13 +4807,11 @@
       <c r="I14" s="10">
         <v>1</v>
       </c>
-      <c r="J14" s="11">
-        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
-      </c>
+      <c r="J14" s="11"/>
       <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>28</v>
       </c>
@@ -3785,21 +4827,17 @@
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
         <v>14</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>29</v>
-      </c>
+      <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10">
         <v>1</v>
       </c>
-      <c r="J15" s="11">
-        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
-      </c>
+      <c r="J15" s="11"/>
       <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
         <v>30</v>
       </c>
@@ -3821,13 +4859,11 @@
       <c r="I16" s="10">
         <v>1</v>
       </c>
-      <c r="J16" s="11">
-        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>14</v>
-      </c>
+      <c r="J16" s="11"/>
       <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
     </row>
-    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>31</v>
       </c>
@@ -3856,8 +4892,9 @@
         <v>14</v>
       </c>
       <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
     </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
@@ -3886,6 +4923,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Updated iteration 6 metrics"
This reverts commit fb8eb915a8d39dad3b6dbaa2e2330cdd42846843.
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
+++ b/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Action</t>
   </si>
@@ -149,12 +149,6 @@
   </si>
   <si>
     <t>Schedule Metrics Score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delayed slightly due to debugging phase, team was unfamiliar with charts. Date/time issue. Date showed NaN. </t>
-  </si>
-  <si>
-    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -386,43 +380,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Century Gothic"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <b val="0"/>
@@ -1217,11 +1175,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-1664024672"/>
-        <c:axId val="-1380287328"/>
+        <c:axId val="-813914064"/>
+        <c:axId val="-813899920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1664024672"/>
+        <c:axId val="-813914064"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1264,7 +1222,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1380287328"/>
+        <c:crossAx val="-813899920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1272,7 +1230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1380287328"/>
+        <c:axId val="-813899920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -1324,7 +1282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1664024672"/>
+        <c:crossAx val="-813914064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -1677,7 +1635,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -1785,11 +1743,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-1380287872"/>
-        <c:axId val="-1380290592"/>
+        <c:axId val="-820918912"/>
+        <c:axId val="-820905856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1380287872"/>
+        <c:axId val="-820918912"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1832,7 +1790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1380290592"/>
+        <c:crossAx val="-820905856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1840,7 +1798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1380290592"/>
+        <c:axId val="-820905856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -1892,7 +1850,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1380287872"/>
+        <c:crossAx val="-820918912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -1974,355 +1932,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-SG" sz="3600">
-                <a:latin typeface="Bebas Neue" panose="020B0606020202050201" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Schedule Metrics</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="35000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Schedule Metrics Tracking'!$J$4:$J$9</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0769230769230769</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.93333333333333335</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="-1380286240"/>
-        <c:axId val="-1380282976"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="-1380286240"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1380282976"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-1380282976"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1380286240"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
   <a:schemeClr val="dk1"/>
@@ -2356,46 +1965,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -3402,508 +2971,6 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3974,100 +3041,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>119062</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>84753</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>149370</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>21648</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>86592</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18876818" y="4572001"/>
-          <a:ext cx="16774824" cy="4723532"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent3">
-            <a:alpha val="8000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:alpha val="13000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="lt1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-SG" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4085,28 +3058,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:L18" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="B3:L18"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="Iteration" dataDxfId="10"/>
-    <tableColumn id="2" name="Planned Start Date" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:K18" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="B3:K18"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Iteration" dataDxfId="9"/>
+    <tableColumn id="2" name="Planned Start Date" dataDxfId="8">
       <calculatedColumnFormula>D3+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Planned End Date" dataDxfId="8">
+    <tableColumn id="3" name="Planned End Date" dataDxfId="7">
       <calculatedColumnFormula>C4+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Duration (Days)" dataDxfId="7">
+    <tableColumn id="6" name="Duration (Days)" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Milestone included" dataDxfId="6"/>
-    <tableColumn id="5" name="Actual Start Date" dataDxfId="5"/>
-    <tableColumn id="7" name="Actual End Date" dataDxfId="4"/>
-    <tableColumn id="8" name="Actual Duration (Days)" dataDxfId="3"/>
-    <tableColumn id="10" name="Schedule Metrics Score" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="4" name="Milestone included" dataDxfId="5"/>
+    <tableColumn id="5" name="Actual Start Date" dataDxfId="4"/>
+    <tableColumn id="7" name="Actual End Date" dataDxfId="3"/>
+    <tableColumn id="8" name="Actual Duration (Days)" dataDxfId="2"/>
+    <tableColumn id="10" name="Schedule Metrics Score" dataDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Action" dataDxfId="1"/>
-    <tableColumn id="11" name="Remarks" dataDxfId="0"/>
+    <tableColumn id="9" name="Action" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4399,10 +3371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L18"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L18" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4417,11 +3389,10 @@
     <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="103.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -4452,11 +3423,8 @@
       <c r="K3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="13" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
@@ -4488,9 +3456,8 @@
       <c r="K4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
@@ -4525,9 +3492,8 @@
       <c r="K5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
@@ -4564,9 +3530,8 @@
       <c r="K6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
@@ -4603,9 +3568,8 @@
       <c r="K7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>21</v>
       </c>
@@ -4635,14 +3599,9 @@
         <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
         <v>0.93333333333333335</v>
       </c>
-      <c r="K8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
@@ -4659,27 +3618,18 @@
         <v>14</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="12">
-        <f t="shared" ref="G9" si="4">H8+1</f>
-        <v>42003</v>
-      </c>
-      <c r="H9" s="12">
-        <f t="shared" ref="H9" si="5">G9+13</f>
-        <v>42016</v>
-      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="10">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J9" s="11">
         <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>1</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
@@ -4701,11 +3651,13 @@
       <c r="I10" s="10">
         <v>1</v>
       </c>
-      <c r="J10" s="11"/>
+      <c r="J10" s="11">
+        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
+        <v>14</v>
+      </c>
       <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
@@ -4727,11 +3679,13 @@
       <c r="I11" s="10">
         <v>1</v>
       </c>
-      <c r="J11" s="11"/>
+      <c r="J11" s="11">
+        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
+        <v>14</v>
+      </c>
       <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>25</v>
       </c>
@@ -4747,19 +3701,19 @@
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
         <v>14</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>29</v>
-      </c>
+      <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10">
         <v>1</v>
       </c>
-      <c r="J12" s="11"/>
+      <c r="J12" s="11">
+        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
+        <v>14</v>
+      </c>
       <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>26</v>
       </c>
@@ -4781,11 +3735,13 @@
       <c r="I13" s="10">
         <v>1</v>
       </c>
-      <c r="J13" s="11"/>
+      <c r="J13" s="11">
+        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
+        <v>14</v>
+      </c>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
         <v>27</v>
       </c>
@@ -4807,11 +3763,13 @@
       <c r="I14" s="10">
         <v>1</v>
       </c>
-      <c r="J14" s="11"/>
+      <c r="J14" s="11">
+        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
+        <v>14</v>
+      </c>
       <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>28</v>
       </c>
@@ -4827,17 +3785,21 @@
         <f>Table1[[#This Row],[Planned End Date]]-Table1[[#This Row],[Planned Start Date]]+1</f>
         <v>14</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10">
         <v>1</v>
       </c>
-      <c r="J15" s="11"/>
+      <c r="J15" s="11">
+        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
+        <v>14</v>
+      </c>
       <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
         <v>30</v>
       </c>
@@ -4859,11 +3821,13 @@
       <c r="I16" s="10">
         <v>1</v>
       </c>
-      <c r="J16" s="11"/>
+      <c r="J16" s="11">
+        <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
+        <v>14</v>
+      </c>
       <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>31</v>
       </c>
@@ -4892,9 +3856,8 @@
         <v>14</v>
       </c>
       <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
@@ -4923,7 +3886,6 @@
         <v>14</v>
       </c>
       <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated meeting minutes and metrics
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
+++ b/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Action</t>
   </si>
@@ -531,14 +531,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -549,16 +549,16 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1424,11 +1424,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="360114848"/>
-        <c:axId val="636728432"/>
+        <c:axId val="1025908080"/>
+        <c:axId val="1025893936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="360114848"/>
+        <c:axId val="1025908080"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1471,7 +1471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636728432"/>
+        <c:crossAx val="1025893936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1479,7 +1479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="636728432"/>
+        <c:axId val="1025893936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -1531,7 +1531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360114848"/>
+        <c:crossAx val="1025908080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -1878,7 +1878,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>15</c:v>
@@ -1992,11 +1992,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="636732240"/>
-        <c:axId val="636731696"/>
+        <c:axId val="1025896112"/>
+        <c:axId val="823141648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="636732240"/>
+        <c:axId val="1025896112"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2039,7 +2039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636731696"/>
+        <c:crossAx val="823141648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2047,7 +2047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="636731696"/>
+        <c:axId val="823141648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -2099,7 +2099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636732240"/>
+        <c:crossAx val="1025896112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -2340,10 +2340,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Schedule Metrics Tracking'!$J$4:$J$11</c:f>
+              <c:f>'Schedule Metrics Tracking'!$J$4:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2354,7 +2354,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0769230769230769</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.93333333333333335</c:v>
@@ -2366,6 +2366,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2382,11 +2385,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="636737136"/>
-        <c:axId val="636730064"/>
+        <c:axId val="1094267504"/>
+        <c:axId val="1094259888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="636737136"/>
+        <c:axId val="1094267504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2428,7 +2431,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636730064"/>
+        <c:crossAx val="1094259888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2436,7 +2439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="636730064"/>
+        <c:axId val="1094259888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2487,7 +2490,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636737136"/>
+        <c:crossAx val="1094267504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4614,8 +4617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AF49" sqref="AF49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4807,11 +4810,11 @@
         <v>41958</v>
       </c>
       <c r="I7" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J7" s="11">
         <f>Table1[[#This Row],[Duration (Days)]]/Table1[[#This Row],[Actual Duration (Days)]]</f>
-        <v>1.0769230769230769</v>
+        <v>1</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>6</v>
@@ -4873,11 +4876,11 @@
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="12">
-        <f t="shared" ref="G9:G11" si="4">H8+1</f>
+        <f t="shared" ref="G9:G12" si="4">H8+1</f>
         <v>42003</v>
       </c>
       <c r="H9" s="12">
-        <f t="shared" ref="H9:H11" si="5">G9+13</f>
+        <f t="shared" ref="H9:H12" si="5">G9+13</f>
         <v>42016</v>
       </c>
       <c r="I9" s="10">
@@ -4987,13 +4990,23 @@
       <c r="F12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="G12" s="12">
+        <f t="shared" si="4"/>
+        <v>42045</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="5"/>
+        <v>42058</v>
+      </c>
       <c r="I12" s="10">
         <v>1</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="10"/>
+      <c r="J12" s="11">
+        <v>1</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="L12" s="10"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5189,100 +5202,100 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:100" ht="36.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="31"/>
-      <c r="AL2" s="31"/>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="31"/>
-      <c r="AQ2" s="31"/>
-      <c r="AR2" s="31"/>
-      <c r="AS2" s="31"/>
-      <c r="AT2" s="31"/>
-      <c r="AU2" s="31"/>
-      <c r="AV2" s="31"/>
-      <c r="AW2" s="31"/>
-      <c r="AX2" s="31"/>
-      <c r="AY2" s="31"/>
-      <c r="AZ2" s="31"/>
-      <c r="BA2" s="31"/>
-      <c r="BB2" s="31"/>
-      <c r="BC2" s="31"/>
-      <c r="BD2" s="31"/>
-      <c r="BE2" s="31"/>
-      <c r="BF2" s="31"/>
-      <c r="BG2" s="31"/>
-      <c r="BH2" s="31"/>
-      <c r="BI2" s="31"/>
-      <c r="BJ2" s="31"/>
-      <c r="BK2" s="31"/>
-      <c r="BL2" s="31"/>
-      <c r="BM2" s="31"/>
-      <c r="BN2" s="31"/>
-      <c r="BO2" s="31"/>
-      <c r="BP2" s="31"/>
-      <c r="BQ2" s="31"/>
-      <c r="BR2" s="31"/>
-      <c r="BS2" s="31"/>
-      <c r="BT2" s="31"/>
-      <c r="BU2" s="31"/>
-      <c r="BV2" s="31"/>
-      <c r="BW2" s="31"/>
-      <c r="BX2" s="31"/>
-      <c r="BY2" s="31"/>
-      <c r="BZ2" s="31"/>
-      <c r="CA2" s="31"/>
-      <c r="CB2" s="31"/>
-      <c r="CC2" s="31"/>
-      <c r="CD2" s="31"/>
-      <c r="CE2" s="31"/>
-      <c r="CF2" s="31"/>
-      <c r="CG2" s="31"/>
-      <c r="CH2" s="31"/>
-      <c r="CI2" s="31"/>
-      <c r="CJ2" s="31"/>
-      <c r="CK2" s="31"/>
-      <c r="CL2" s="31"/>
-      <c r="CM2" s="31"/>
-      <c r="CN2" s="31"/>
-      <c r="CO2" s="32"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
+      <c r="BA2" s="37"/>
+      <c r="BB2" s="37"/>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+      <c r="BF2" s="37"/>
+      <c r="BG2" s="37"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="37"/>
+      <c r="BK2" s="37"/>
+      <c r="BL2" s="37"/>
+      <c r="BM2" s="37"/>
+      <c r="BN2" s="37"/>
+      <c r="BO2" s="37"/>
+      <c r="BP2" s="37"/>
+      <c r="BQ2" s="37"/>
+      <c r="BR2" s="37"/>
+      <c r="BS2" s="37"/>
+      <c r="BT2" s="37"/>
+      <c r="BU2" s="37"/>
+      <c r="BV2" s="37"/>
+      <c r="BW2" s="37"/>
+      <c r="BX2" s="37"/>
+      <c r="BY2" s="37"/>
+      <c r="BZ2" s="37"/>
+      <c r="CA2" s="37"/>
+      <c r="CB2" s="37"/>
+      <c r="CC2" s="37"/>
+      <c r="CD2" s="37"/>
+      <c r="CE2" s="37"/>
+      <c r="CF2" s="37"/>
+      <c r="CG2" s="37"/>
+      <c r="CH2" s="37"/>
+      <c r="CI2" s="37"/>
+      <c r="CJ2" s="37"/>
+      <c r="CK2" s="37"/>
+      <c r="CL2" s="37"/>
+      <c r="CM2" s="37"/>
+      <c r="CN2" s="37"/>
+      <c r="CO2" s="38"/>
     </row>
     <row r="3" spans="2:100" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="15"/>
@@ -5389,13 +5402,13 @@
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
       <c r="I4" s="35"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
       <c r="S4" s="17"/>
@@ -6042,20 +6055,20 @@
       <c r="CF10" s="20"/>
       <c r="CG10" s="20"/>
       <c r="CH10" s="20"/>
-      <c r="CI10" s="38"/>
-      <c r="CJ10" s="38"/>
-      <c r="CK10" s="38"/>
-      <c r="CL10" s="38"/>
-      <c r="CM10" s="38"/>
-      <c r="CN10" s="38"/>
-      <c r="CO10" s="39"/>
-      <c r="CP10" s="37"/>
-      <c r="CQ10" s="37"/>
-      <c r="CR10" s="37"/>
-      <c r="CS10" s="37"/>
-      <c r="CT10" s="37"/>
-      <c r="CU10" s="37"/>
-      <c r="CV10" s="37"/>
+      <c r="CI10" s="31"/>
+      <c r="CJ10" s="31"/>
+      <c r="CK10" s="31"/>
+      <c r="CL10" s="31"/>
+      <c r="CM10" s="31"/>
+      <c r="CN10" s="31"/>
+      <c r="CO10" s="32"/>
+      <c r="CP10" s="30"/>
+      <c r="CQ10" s="30"/>
+      <c r="CR10" s="30"/>
+      <c r="CS10" s="30"/>
+      <c r="CT10" s="30"/>
+      <c r="CU10" s="30"/>
+      <c r="CV10" s="30"/>
     </row>
     <row r="11" spans="2:100" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="15"/>
@@ -6724,100 +6737,100 @@
       <c r="CO17" s="21"/>
     </row>
     <row r="18" spans="2:93" ht="36.75" x14ac:dyDescent="0.6">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="31"/>
-      <c r="Z18" s="31"/>
-      <c r="AA18" s="31"/>
-      <c r="AB18" s="31"/>
-      <c r="AC18" s="31"/>
-      <c r="AD18" s="31"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
-      <c r="AI18" s="31"/>
-      <c r="AJ18" s="31"/>
-      <c r="AK18" s="31"/>
-      <c r="AL18" s="31"/>
-      <c r="AM18" s="31"/>
-      <c r="AN18" s="31"/>
-      <c r="AO18" s="31"/>
-      <c r="AP18" s="31"/>
-      <c r="AQ18" s="31"/>
-      <c r="AR18" s="31"/>
-      <c r="AS18" s="31"/>
-      <c r="AT18" s="31"/>
-      <c r="AU18" s="31"/>
-      <c r="AV18" s="31"/>
-      <c r="AW18" s="31"/>
-      <c r="AX18" s="31"/>
-      <c r="AY18" s="31"/>
-      <c r="AZ18" s="31"/>
-      <c r="BA18" s="31"/>
-      <c r="BB18" s="31"/>
-      <c r="BC18" s="31"/>
-      <c r="BD18" s="31"/>
-      <c r="BE18" s="31"/>
-      <c r="BF18" s="31"/>
-      <c r="BG18" s="31"/>
-      <c r="BH18" s="31"/>
-      <c r="BI18" s="31"/>
-      <c r="BJ18" s="31"/>
-      <c r="BK18" s="31"/>
-      <c r="BL18" s="31"/>
-      <c r="BM18" s="31"/>
-      <c r="BN18" s="31"/>
-      <c r="BO18" s="31"/>
-      <c r="BP18" s="31"/>
-      <c r="BQ18" s="31"/>
-      <c r="BR18" s="31"/>
-      <c r="BS18" s="31"/>
-      <c r="BT18" s="31"/>
-      <c r="BU18" s="31"/>
-      <c r="BV18" s="31"/>
-      <c r="BW18" s="31"/>
-      <c r="BX18" s="31"/>
-      <c r="BY18" s="31"/>
-      <c r="BZ18" s="31"/>
-      <c r="CA18" s="31"/>
-      <c r="CB18" s="31"/>
-      <c r="CC18" s="31"/>
-      <c r="CD18" s="31"/>
-      <c r="CE18" s="31"/>
-      <c r="CF18" s="31"/>
-      <c r="CG18" s="31"/>
-      <c r="CH18" s="31"/>
-      <c r="CI18" s="31"/>
-      <c r="CJ18" s="31"/>
-      <c r="CK18" s="31"/>
-      <c r="CL18" s="31"/>
-      <c r="CM18" s="31"/>
-      <c r="CN18" s="31"/>
-      <c r="CO18" s="32"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="37"/>
+      <c r="W18" s="37"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="37"/>
+      <c r="Z18" s="37"/>
+      <c r="AA18" s="37"/>
+      <c r="AB18" s="37"/>
+      <c r="AC18" s="37"/>
+      <c r="AD18" s="37"/>
+      <c r="AE18" s="37"/>
+      <c r="AF18" s="37"/>
+      <c r="AG18" s="37"/>
+      <c r="AH18" s="37"/>
+      <c r="AI18" s="37"/>
+      <c r="AJ18" s="37"/>
+      <c r="AK18" s="37"/>
+      <c r="AL18" s="37"/>
+      <c r="AM18" s="37"/>
+      <c r="AN18" s="37"/>
+      <c r="AO18" s="37"/>
+      <c r="AP18" s="37"/>
+      <c r="AQ18" s="37"/>
+      <c r="AR18" s="37"/>
+      <c r="AS18" s="37"/>
+      <c r="AT18" s="37"/>
+      <c r="AU18" s="37"/>
+      <c r="AV18" s="37"/>
+      <c r="AW18" s="37"/>
+      <c r="AX18" s="37"/>
+      <c r="AY18" s="37"/>
+      <c r="AZ18" s="37"/>
+      <c r="BA18" s="37"/>
+      <c r="BB18" s="37"/>
+      <c r="BC18" s="37"/>
+      <c r="BD18" s="37"/>
+      <c r="BE18" s="37"/>
+      <c r="BF18" s="37"/>
+      <c r="BG18" s="37"/>
+      <c r="BH18" s="37"/>
+      <c r="BI18" s="37"/>
+      <c r="BJ18" s="37"/>
+      <c r="BK18" s="37"/>
+      <c r="BL18" s="37"/>
+      <c r="BM18" s="37"/>
+      <c r="BN18" s="37"/>
+      <c r="BO18" s="37"/>
+      <c r="BP18" s="37"/>
+      <c r="BQ18" s="37"/>
+      <c r="BR18" s="37"/>
+      <c r="BS18" s="37"/>
+      <c r="BT18" s="37"/>
+      <c r="BU18" s="37"/>
+      <c r="BV18" s="37"/>
+      <c r="BW18" s="37"/>
+      <c r="BX18" s="37"/>
+      <c r="BY18" s="37"/>
+      <c r="BZ18" s="37"/>
+      <c r="CA18" s="37"/>
+      <c r="CB18" s="37"/>
+      <c r="CC18" s="37"/>
+      <c r="CD18" s="37"/>
+      <c r="CE18" s="37"/>
+      <c r="CF18" s="37"/>
+      <c r="CG18" s="37"/>
+      <c r="CH18" s="37"/>
+      <c r="CI18" s="37"/>
+      <c r="CJ18" s="37"/>
+      <c r="CK18" s="37"/>
+      <c r="CL18" s="37"/>
+      <c r="CM18" s="37"/>
+      <c r="CN18" s="37"/>
+      <c r="CO18" s="38"/>
     </row>
     <row r="19" spans="2:93" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="15"/>
@@ -6924,13 +6937,13 @@
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
       <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
@@ -8057,17 +8070,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="CP10:CV10"/>
-    <mergeCell ref="CI10:CO10"/>
-    <mergeCell ref="AS10:AY10"/>
-    <mergeCell ref="AZ11:BF11"/>
-    <mergeCell ref="BG12:BM12"/>
-    <mergeCell ref="AE24:AK24"/>
-    <mergeCell ref="AL25:AR25"/>
-    <mergeCell ref="AS26:AY26"/>
-    <mergeCell ref="BN13:BT13"/>
-    <mergeCell ref="BU14:CA14"/>
-    <mergeCell ref="B18:CO18"/>
     <mergeCell ref="B2:CO2"/>
     <mergeCell ref="J21:P21"/>
     <mergeCell ref="Q22:W22"/>
@@ -8081,6 +8083,17 @@
     <mergeCell ref="Q6:W6"/>
     <mergeCell ref="X7:AD7"/>
     <mergeCell ref="AE8:AK8"/>
+    <mergeCell ref="AE24:AK24"/>
+    <mergeCell ref="AL25:AR25"/>
+    <mergeCell ref="AS26:AY26"/>
+    <mergeCell ref="BN13:BT13"/>
+    <mergeCell ref="BU14:CA14"/>
+    <mergeCell ref="B18:CO18"/>
+    <mergeCell ref="CP10:CV10"/>
+    <mergeCell ref="CI10:CO10"/>
+    <mergeCell ref="AS10:AY10"/>
+    <mergeCell ref="AZ11:BF11"/>
+    <mergeCell ref="BG12:BM12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
remove scenario attributes after case creation done
</commit_message>
<xml_diff>
--- a/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
+++ b/Documents/Project Management/Metrics/Schedule Metrics/Schedule Metrics Tracking.xlsx
@@ -546,15 +546,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -565,6 +556,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1430,11 +1430,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="93207456"/>
-        <c:axId val="93208000"/>
+        <c:axId val="-585062256"/>
+        <c:axId val="-585061712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93207456"/>
+        <c:axId val="-585062256"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1477,7 +1477,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93208000"/>
+        <c:crossAx val="-585061712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1485,7 +1485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93208000"/>
+        <c:axId val="-585061712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -1537,7 +1537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93207456"/>
+        <c:crossAx val="-585062256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -1907,7 +1907,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
@@ -1997,11 +1997,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="93213440"/>
-        <c:axId val="93208544"/>
+        <c:axId val="-721090096"/>
+        <c:axId val="-721089552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93213440"/>
+        <c:axId val="-721090096"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2044,7 +2044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93208544"/>
+        <c:crossAx val="-721089552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2052,7 +2052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93208544"/>
+        <c:axId val="-721089552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="41904"/>
@@ -2104,7 +2104,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93213440"/>
+        <c:crossAx val="-721090096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="14"/>
@@ -2227,7 +2227,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2323,7 +2322,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2392,11 +2390,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="93210176"/>
-        <c:axId val="93210720"/>
+        <c:axId val="-438279536"/>
+        <c:axId val="-438278992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93210176"/>
+        <c:axId val="-438279536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2438,7 +2436,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93210720"/>
+        <c:crossAx val="-438278992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2446,7 +2444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93210720"/>
+        <c:axId val="-438278992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2495,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93210176"/>
+        <c:crossAx val="-438279536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4624,8 +4622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4883,12 +4881,11 @@
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="12">
-        <f t="shared" ref="G9:G12" si="4">H8+1</f>
-        <v>42003</v>
+        <v>42002</v>
       </c>
       <c r="H9" s="12">
-        <f t="shared" ref="H9:H14" si="5">G9+13</f>
-        <v>42016</v>
+        <f t="shared" ref="H9:H13" si="4">G9+13</f>
+        <v>42015</v>
       </c>
       <c r="I9" s="10">
         <v>14</v>
@@ -4922,12 +4919,12 @@
         <v>42</v>
       </c>
       <c r="G10" s="12">
+        <f t="shared" ref="G9:G12" si="5">H9+1</f>
+        <v>42016</v>
+      </c>
+      <c r="H10" s="12">
         <f t="shared" si="4"/>
-        <v>42017</v>
-      </c>
-      <c r="H10" s="12">
-        <f t="shared" si="5"/>
-        <v>42030</v>
+        <v>42029</v>
       </c>
       <c r="I10" s="10">
         <v>14</v>
@@ -4961,12 +4958,12 @@
         <v>43</v>
       </c>
       <c r="G11" s="12">
+        <f t="shared" si="5"/>
+        <v>42030</v>
+      </c>
+      <c r="H11" s="12">
         <f t="shared" si="4"/>
-        <v>42031</v>
-      </c>
-      <c r="H11" s="12">
-        <f t="shared" si="5"/>
-        <v>42044</v>
+        <v>42043</v>
       </c>
       <c r="I11" s="10">
         <v>14</v>
@@ -5000,11 +4997,11 @@
         <v>29</v>
       </c>
       <c r="G12" s="12">
-        <f t="shared" si="4"/>
-        <v>42045</v>
+        <f t="shared" si="5"/>
+        <v>42044</v>
       </c>
       <c r="H12" s="12">
-        <f>G12+12</f>
+        <f>G12+13</f>
         <v>42057</v>
       </c>
       <c r="I12" s="10">
@@ -5043,7 +5040,7 @@
         <v>42058</v>
       </c>
       <c r="H13" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>42071</v>
       </c>
       <c r="I13" s="10">
@@ -5119,9 +5116,12 @@
       <c r="G15" s="12">
         <v>42087</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="12">
+        <f>Table1[[#This Row],[Actual Start Date]]+13</f>
+        <v>42100</v>
+      </c>
       <c r="I15" s="10">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="10"/>
@@ -5240,100 +5240,100 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:100" ht="36.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
-      <c r="AQ2" s="37"/>
-      <c r="AR2" s="37"/>
-      <c r="AS2" s="37"/>
-      <c r="AT2" s="37"/>
-      <c r="AU2" s="37"/>
-      <c r="AV2" s="37"/>
-      <c r="AW2" s="37"/>
-      <c r="AX2" s="37"/>
-      <c r="AY2" s="37"/>
-      <c r="AZ2" s="37"/>
-      <c r="BA2" s="37"/>
-      <c r="BB2" s="37"/>
-      <c r="BC2" s="37"/>
-      <c r="BD2" s="37"/>
-      <c r="BE2" s="37"/>
-      <c r="BF2" s="37"/>
-      <c r="BG2" s="37"/>
-      <c r="BH2" s="37"/>
-      <c r="BI2" s="37"/>
-      <c r="BJ2" s="37"/>
-      <c r="BK2" s="37"/>
-      <c r="BL2" s="37"/>
-      <c r="BM2" s="37"/>
-      <c r="BN2" s="37"/>
-      <c r="BO2" s="37"/>
-      <c r="BP2" s="37"/>
-      <c r="BQ2" s="37"/>
-      <c r="BR2" s="37"/>
-      <c r="BS2" s="37"/>
-      <c r="BT2" s="37"/>
-      <c r="BU2" s="37"/>
-      <c r="BV2" s="37"/>
-      <c r="BW2" s="37"/>
-      <c r="BX2" s="37"/>
-      <c r="BY2" s="37"/>
-      <c r="BZ2" s="37"/>
-      <c r="CA2" s="37"/>
-      <c r="CB2" s="37"/>
-      <c r="CC2" s="37"/>
-      <c r="CD2" s="37"/>
-      <c r="CE2" s="37"/>
-      <c r="CF2" s="37"/>
-      <c r="CG2" s="37"/>
-      <c r="CH2" s="37"/>
-      <c r="CI2" s="37"/>
-      <c r="CJ2" s="37"/>
-      <c r="CK2" s="37"/>
-      <c r="CL2" s="37"/>
-      <c r="CM2" s="37"/>
-      <c r="CN2" s="37"/>
-      <c r="CO2" s="38"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="34"/>
+      <c r="AT2" s="34"/>
+      <c r="AU2" s="34"/>
+      <c r="AV2" s="34"/>
+      <c r="AW2" s="34"/>
+      <c r="AX2" s="34"/>
+      <c r="AY2" s="34"/>
+      <c r="AZ2" s="34"/>
+      <c r="BA2" s="34"/>
+      <c r="BB2" s="34"/>
+      <c r="BC2" s="34"/>
+      <c r="BD2" s="34"/>
+      <c r="BE2" s="34"/>
+      <c r="BF2" s="34"/>
+      <c r="BG2" s="34"/>
+      <c r="BH2" s="34"/>
+      <c r="BI2" s="34"/>
+      <c r="BJ2" s="34"/>
+      <c r="BK2" s="34"/>
+      <c r="BL2" s="34"/>
+      <c r="BM2" s="34"/>
+      <c r="BN2" s="34"/>
+      <c r="BO2" s="34"/>
+      <c r="BP2" s="34"/>
+      <c r="BQ2" s="34"/>
+      <c r="BR2" s="34"/>
+      <c r="BS2" s="34"/>
+      <c r="BT2" s="34"/>
+      <c r="BU2" s="34"/>
+      <c r="BV2" s="34"/>
+      <c r="BW2" s="34"/>
+      <c r="BX2" s="34"/>
+      <c r="BY2" s="34"/>
+      <c r="BZ2" s="34"/>
+      <c r="CA2" s="34"/>
+      <c r="CB2" s="34"/>
+      <c r="CC2" s="34"/>
+      <c r="CD2" s="34"/>
+      <c r="CE2" s="34"/>
+      <c r="CF2" s="34"/>
+      <c r="CG2" s="34"/>
+      <c r="CH2" s="34"/>
+      <c r="CI2" s="34"/>
+      <c r="CJ2" s="34"/>
+      <c r="CK2" s="34"/>
+      <c r="CL2" s="34"/>
+      <c r="CM2" s="34"/>
+      <c r="CN2" s="34"/>
+      <c r="CO2" s="35"/>
     </row>
     <row r="3" spans="2:100" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="15"/>
@@ -5440,13 +5440,13 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
       <c r="I4" s="32"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
       <c r="S4" s="17"/>
@@ -6093,20 +6093,20 @@
       <c r="CF10" s="20"/>
       <c r="CG10" s="20"/>
       <c r="CH10" s="20"/>
-      <c r="CI10" s="34"/>
-      <c r="CJ10" s="34"/>
-      <c r="CK10" s="34"/>
-      <c r="CL10" s="34"/>
-      <c r="CM10" s="34"/>
-      <c r="CN10" s="34"/>
-      <c r="CO10" s="35"/>
-      <c r="CP10" s="33"/>
-      <c r="CQ10" s="33"/>
-      <c r="CR10" s="33"/>
-      <c r="CS10" s="33"/>
-      <c r="CT10" s="33"/>
-      <c r="CU10" s="33"/>
-      <c r="CV10" s="33"/>
+      <c r="CI10" s="38"/>
+      <c r="CJ10" s="38"/>
+      <c r="CK10" s="38"/>
+      <c r="CL10" s="38"/>
+      <c r="CM10" s="38"/>
+      <c r="CN10" s="38"/>
+      <c r="CO10" s="39"/>
+      <c r="CP10" s="37"/>
+      <c r="CQ10" s="37"/>
+      <c r="CR10" s="37"/>
+      <c r="CS10" s="37"/>
+      <c r="CT10" s="37"/>
+      <c r="CU10" s="37"/>
+      <c r="CV10" s="37"/>
     </row>
     <row r="11" spans="2:100" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="15"/>
@@ -6775,100 +6775,100 @@
       <c r="CO17" s="21"/>
     </row>
     <row r="18" spans="2:93" ht="36.75" x14ac:dyDescent="0.6">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="37"/>
-      <c r="AA18" s="37"/>
-      <c r="AB18" s="37"/>
-      <c r="AC18" s="37"/>
-      <c r="AD18" s="37"/>
-      <c r="AE18" s="37"/>
-      <c r="AF18" s="37"/>
-      <c r="AG18" s="37"/>
-      <c r="AH18" s="37"/>
-      <c r="AI18" s="37"/>
-      <c r="AJ18" s="37"/>
-      <c r="AK18" s="37"/>
-      <c r="AL18" s="37"/>
-      <c r="AM18" s="37"/>
-      <c r="AN18" s="37"/>
-      <c r="AO18" s="37"/>
-      <c r="AP18" s="37"/>
-      <c r="AQ18" s="37"/>
-      <c r="AR18" s="37"/>
-      <c r="AS18" s="37"/>
-      <c r="AT18" s="37"/>
-      <c r="AU18" s="37"/>
-      <c r="AV18" s="37"/>
-      <c r="AW18" s="37"/>
-      <c r="AX18" s="37"/>
-      <c r="AY18" s="37"/>
-      <c r="AZ18" s="37"/>
-      <c r="BA18" s="37"/>
-      <c r="BB18" s="37"/>
-      <c r="BC18" s="37"/>
-      <c r="BD18" s="37"/>
-      <c r="BE18" s="37"/>
-      <c r="BF18" s="37"/>
-      <c r="BG18" s="37"/>
-      <c r="BH18" s="37"/>
-      <c r="BI18" s="37"/>
-      <c r="BJ18" s="37"/>
-      <c r="BK18" s="37"/>
-      <c r="BL18" s="37"/>
-      <c r="BM18" s="37"/>
-      <c r="BN18" s="37"/>
-      <c r="BO18" s="37"/>
-      <c r="BP18" s="37"/>
-      <c r="BQ18" s="37"/>
-      <c r="BR18" s="37"/>
-      <c r="BS18" s="37"/>
-      <c r="BT18" s="37"/>
-      <c r="BU18" s="37"/>
-      <c r="BV18" s="37"/>
-      <c r="BW18" s="37"/>
-      <c r="BX18" s="37"/>
-      <c r="BY18" s="37"/>
-      <c r="BZ18" s="37"/>
-      <c r="CA18" s="37"/>
-      <c r="CB18" s="37"/>
-      <c r="CC18" s="37"/>
-      <c r="CD18" s="37"/>
-      <c r="CE18" s="37"/>
-      <c r="CF18" s="37"/>
-      <c r="CG18" s="37"/>
-      <c r="CH18" s="37"/>
-      <c r="CI18" s="37"/>
-      <c r="CJ18" s="37"/>
-      <c r="CK18" s="37"/>
-      <c r="CL18" s="37"/>
-      <c r="CM18" s="37"/>
-      <c r="CN18" s="37"/>
-      <c r="CO18" s="38"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="34"/>
+      <c r="X18" s="34"/>
+      <c r="Y18" s="34"/>
+      <c r="Z18" s="34"/>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="34"/>
+      <c r="AC18" s="34"/>
+      <c r="AD18" s="34"/>
+      <c r="AE18" s="34"/>
+      <c r="AF18" s="34"/>
+      <c r="AG18" s="34"/>
+      <c r="AH18" s="34"/>
+      <c r="AI18" s="34"/>
+      <c r="AJ18" s="34"/>
+      <c r="AK18" s="34"/>
+      <c r="AL18" s="34"/>
+      <c r="AM18" s="34"/>
+      <c r="AN18" s="34"/>
+      <c r="AO18" s="34"/>
+      <c r="AP18" s="34"/>
+      <c r="AQ18" s="34"/>
+      <c r="AR18" s="34"/>
+      <c r="AS18" s="34"/>
+      <c r="AT18" s="34"/>
+      <c r="AU18" s="34"/>
+      <c r="AV18" s="34"/>
+      <c r="AW18" s="34"/>
+      <c r="AX18" s="34"/>
+      <c r="AY18" s="34"/>
+      <c r="AZ18" s="34"/>
+      <c r="BA18" s="34"/>
+      <c r="BB18" s="34"/>
+      <c r="BC18" s="34"/>
+      <c r="BD18" s="34"/>
+      <c r="BE18" s="34"/>
+      <c r="BF18" s="34"/>
+      <c r="BG18" s="34"/>
+      <c r="BH18" s="34"/>
+      <c r="BI18" s="34"/>
+      <c r="BJ18" s="34"/>
+      <c r="BK18" s="34"/>
+      <c r="BL18" s="34"/>
+      <c r="BM18" s="34"/>
+      <c r="BN18" s="34"/>
+      <c r="BO18" s="34"/>
+      <c r="BP18" s="34"/>
+      <c r="BQ18" s="34"/>
+      <c r="BR18" s="34"/>
+      <c r="BS18" s="34"/>
+      <c r="BT18" s="34"/>
+      <c r="BU18" s="34"/>
+      <c r="BV18" s="34"/>
+      <c r="BW18" s="34"/>
+      <c r="BX18" s="34"/>
+      <c r="BY18" s="34"/>
+      <c r="BZ18" s="34"/>
+      <c r="CA18" s="34"/>
+      <c r="CB18" s="34"/>
+      <c r="CC18" s="34"/>
+      <c r="CD18" s="34"/>
+      <c r="CE18" s="34"/>
+      <c r="CF18" s="34"/>
+      <c r="CG18" s="34"/>
+      <c r="CH18" s="34"/>
+      <c r="CI18" s="34"/>
+      <c r="CJ18" s="34"/>
+      <c r="CK18" s="34"/>
+      <c r="CL18" s="34"/>
+      <c r="CM18" s="34"/>
+      <c r="CN18" s="34"/>
+      <c r="CO18" s="35"/>
     </row>
     <row r="19" spans="2:93" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="15"/>
@@ -6975,13 +6975,13 @@
       <c r="G20" s="31"/>
       <c r="H20" s="31"/>
       <c r="I20" s="32"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
@@ -8114,12 +8114,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="AS26:AY26"/>
-    <mergeCell ref="BN13:BT13"/>
-    <mergeCell ref="BU14:CA14"/>
-    <mergeCell ref="B18:CO18"/>
-    <mergeCell ref="AE24:AK24"/>
-    <mergeCell ref="AL25:AR25"/>
+    <mergeCell ref="AZ27:BF27"/>
+    <mergeCell ref="BG28:BM28"/>
+    <mergeCell ref="BN29:BT29"/>
+    <mergeCell ref="CP10:CV10"/>
+    <mergeCell ref="CI10:CO10"/>
     <mergeCell ref="B2:CO2"/>
     <mergeCell ref="J21:P21"/>
     <mergeCell ref="Q22:W22"/>
@@ -8136,11 +8135,12 @@
     <mergeCell ref="AZ11:BF11"/>
     <mergeCell ref="BG12:BM12"/>
     <mergeCell ref="AE8:AK8"/>
-    <mergeCell ref="AZ27:BF27"/>
-    <mergeCell ref="BG28:BM28"/>
-    <mergeCell ref="BN29:BT29"/>
-    <mergeCell ref="CP10:CV10"/>
-    <mergeCell ref="CI10:CO10"/>
+    <mergeCell ref="AS26:AY26"/>
+    <mergeCell ref="BN13:BT13"/>
+    <mergeCell ref="BU14:CA14"/>
+    <mergeCell ref="B18:CO18"/>
+    <mergeCell ref="AE24:AK24"/>
+    <mergeCell ref="AL25:AR25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>